<commit_message>
Update IP - EX 42 - Procuras indice e corresp (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 42 - Procuras indice e corresp (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 42 - Procuras indice e corresp (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{188DCA69-09B9-4F5E-A509-9263DB09F431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACF3262-77F8-4487-BFFE-E3CAE51199ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -31,8 +31,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
   <si>
     <t>INDICE</t>
   </si>
@@ -1244,7 +1266,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1540,9 +1562,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1593,6 +1612,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2159,11 +2190,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2318,7 +2353,9 @@
       <c r="J12" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="99"/>
+      <c r="K12" s="99" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="36" t="s">
@@ -2330,11 +2367,15 @@
       <c r="J13" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="99"/>
+      <c r="K13" s="99" t="s">
+        <v>41</v>
+      </c>
       <c r="M13" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="N13" s="99"/>
+      <c r="N13" s="99">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="36" t="s">
@@ -2510,6 +2551,14 @@
     <mergeCell ref="B2:Q6"/>
     <mergeCell ref="B9:Q9"/>
   </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12" xr:uid="{1F9450EA-F501-4A1C-A73F-77C294856EB5}">
+      <formula1>$J$17:$J$24</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13" xr:uid="{5A61EF95-A7BE-4F49-8811-3ACC4E436374}">
+      <formula1>$K$16:$N$16</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2519,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63:F63"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64:F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,7 +2808,10 @@
       <c r="B16" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="87"/>
+      <c r="C16" s="87" t="str" cm="1">
+        <f t="array" ref="C16">INDEX(B10:F13,A12,D9)</f>
+        <v>BUSCAR</v>
+      </c>
       <c r="G16" s="92">
         <v>7</v>
       </c>
@@ -2787,7 +2839,10 @@
       <c r="H20" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="87"/>
+      <c r="I20" s="87" t="str" cm="1">
+        <f t="array" ref="I20">INDEX(H10:I18,G16,H9)</f>
+        <v>BUSCAR</v>
+      </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="54" t="s">
@@ -2819,6 +2874,9 @@
       <c r="J24" t="s">
         <v>8</v>
       </c>
+      <c r="K24" s="25">
+        <v>1</v>
+      </c>
       <c r="L24" s="68"/>
       <c r="N24" s="1" t="s">
         <v>5</v>
@@ -2834,8 +2892,23 @@
       <c r="D25" s="100">
         <v>3</v>
       </c>
+      <c r="E25" s="100">
+        <v>4</v>
+      </c>
+      <c r="F25" s="100">
+        <v>5</v>
+      </c>
+      <c r="G25" s="100">
+        <v>6</v>
+      </c>
+      <c r="H25" s="100">
+        <v>7</v>
+      </c>
       <c r="J25" s="71" t="s">
         <v>3</v>
+      </c>
+      <c r="K25" s="156">
+        <v>2</v>
       </c>
       <c r="L25" s="71" t="s">
         <v>3</v>
@@ -2847,34 +2920,55 @@
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="65"/>
       <c r="C26" s="66"/>
-      <c r="D26" s="71" t="s">
+      <c r="D26" s="66"/>
+      <c r="E26" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="66"/>
       <c r="F26" s="66"/>
       <c r="G26" s="66"/>
       <c r="H26" s="67"/>
+      <c r="K26" s="25">
+        <v>3</v>
+      </c>
       <c r="L26" s="69"/>
     </row>
     <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="156">
+        <v>4</v>
+      </c>
       <c r="L27" s="69"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D28" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="87"/>
+      <c r="E28" s="87">
+        <f>MATCH(C24,B26:H26,0)</f>
+        <v>4</v>
+      </c>
+      <c r="K28" s="25">
+        <v>5</v>
+      </c>
       <c r="L28" s="69"/>
       <c r="N28" s="20"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K29" s="156">
+        <v>6</v>
+      </c>
       <c r="L29" s="69"/>
       <c r="N29" s="20"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K30" s="25">
+        <v>7</v>
+      </c>
       <c r="L30" s="69"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K31" s="156">
+        <v>8</v>
+      </c>
       <c r="L31" s="70"/>
     </row>
     <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2882,7 +2976,10 @@
       <c r="K33" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="L33" s="87"/>
+      <c r="L33" s="87">
+        <f>MATCH(J25,L24:L31,0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="54" t="s">
@@ -3062,7 +3159,9 @@
       <c r="M43" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="N43" s="87"/>
+      <c r="N43" s="87">
+        <v>2</v>
+      </c>
     </row>
     <row r="44" spans="2:17" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:17" x14ac:dyDescent="0.25">
@@ -3092,7 +3191,10 @@
       <c r="C47" s="119"/>
       <c r="D47" s="119"/>
       <c r="E47" s="119"/>
-      <c r="F47" s="120"/>
+      <c r="F47" s="120" cm="1">
+        <f t="array" ref="F47">INDEX(C40:F43,N43,N49)</f>
+        <v>3</v>
+      </c>
       <c r="H47" s="117"/>
       <c r="I47" s="22">
         <v>2</v>
@@ -3137,7 +3239,9 @@
       <c r="M49" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="N49" s="87"/>
+      <c r="N49" s="87">
+        <v>3</v>
+      </c>
     </row>
     <row r="52" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B52" s="54" t="s">
@@ -3193,17 +3297,20 @@
       <c r="H56" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J56" s="126"/>
+      <c r="J56" s="126">
+        <f>INDEX(E57:H60,MATCH(D63,B57:B60,0),MATCH(D64,E56:H56,0))</f>
+        <v>6.3</v>
+      </c>
       <c r="K56" s="127"/>
       <c r="L56" s="127"/>
       <c r="M56" s="128"/>
     </row>
     <row r="57" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B57" s="139" t="s">
+      <c r="B57" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="140"/>
-      <c r="D57" s="141"/>
+      <c r="C57" s="158"/>
+      <c r="D57" s="159"/>
       <c r="E57" s="21">
         <v>1.5</v>
       </c>
@@ -3225,11 +3332,11 @@
       <c r="M57" s="131"/>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B58" s="139" t="s">
+      <c r="B58" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="140"/>
-      <c r="D58" s="141"/>
+      <c r="C58" s="158"/>
+      <c r="D58" s="159"/>
       <c r="E58" s="21">
         <v>2</v>
       </c>
@@ -3251,11 +3358,11 @@
       <c r="M58" s="131"/>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B59" s="139" t="s">
+      <c r="B59" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="140"/>
-      <c r="D59" s="141"/>
+      <c r="C59" s="158"/>
+      <c r="D59" s="159"/>
       <c r="E59" s="21">
         <v>3.2</v>
       </c>
@@ -3277,11 +3384,11 @@
       <c r="M59" s="131"/>
     </row>
     <row r="60" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B60" s="139" t="s">
+      <c r="B60" s="157" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="140"/>
-      <c r="D60" s="141"/>
+      <c r="C60" s="158"/>
+      <c r="D60" s="159"/>
       <c r="E60" s="21">
         <v>4.8</v>
       </c>
@@ -3312,7 +3419,7 @@
         <v>28</v>
       </c>
       <c r="D63" s="124" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E63" s="124"/>
       <c r="F63" s="124"/>
@@ -3358,6 +3465,20 @@
     <mergeCell ref="J48:L48"/>
     <mergeCell ref="J49:L49"/>
   </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N43" xr:uid="{B6650E78-D43A-4EDB-9576-7F3E97D42508}">
+      <formula1>$I$40:$I$43</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N49" xr:uid="{7038109F-CDE2-44B2-B9A3-9B43411CF68C}">
+      <formula1>$I$46:$I$49</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D63:F63" xr:uid="{12A91625-3A5C-4A53-BB03-ABFE6E28DEEF}">
+      <formula1>$B$57:$B$60</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D64:F64" xr:uid="{A3075FAD-A08C-472F-B364-DABE8B70FA85}">
+      <formula1>$E$56:$H$56</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3380,97 +3501,97 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="142" t="str">
+      <c r="B2" s="139" t="str">
         <f>CONTEÚDO!B2</f>
         <v>ÍNDICE e CORRESP</v>
       </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
-      <c r="O2" s="143"/>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="144"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="140"/>
+      <c r="M2" s="140"/>
+      <c r="N2" s="140"/>
+      <c r="O2" s="140"/>
+      <c r="P2" s="140"/>
+      <c r="Q2" s="141"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="145"/>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="146"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="146"/>
-      <c r="O3" s="146"/>
-      <c r="P3" s="146"/>
-      <c r="Q3" s="147"/>
+      <c r="B3" s="142"/>
+      <c r="C3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="143"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="143"/>
+      <c r="O3" s="143"/>
+      <c r="P3" s="143"/>
+      <c r="Q3" s="144"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="145"/>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-      <c r="J4" s="146"/>
-      <c r="K4" s="146"/>
-      <c r="L4" s="146"/>
-      <c r="M4" s="146"/>
-      <c r="N4" s="146"/>
-      <c r="O4" s="146"/>
-      <c r="P4" s="146"/>
-      <c r="Q4" s="147"/>
+      <c r="B4" s="142"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="143"/>
+      <c r="L4" s="143"/>
+      <c r="M4" s="143"/>
+      <c r="N4" s="143"/>
+      <c r="O4" s="143"/>
+      <c r="P4" s="143"/>
+      <c r="Q4" s="144"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="145"/>
-      <c r="C5" s="146"/>
-      <c r="D5" s="146"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="146"/>
-      <c r="H5" s="146"/>
-      <c r="I5" s="146"/>
-      <c r="J5" s="146"/>
-      <c r="K5" s="146"/>
-      <c r="L5" s="146"/>
-      <c r="M5" s="146"/>
-      <c r="N5" s="146"/>
-      <c r="O5" s="146"/>
-      <c r="P5" s="146"/>
-      <c r="Q5" s="147"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="143"/>
+      <c r="N5" s="143"/>
+      <c r="O5" s="143"/>
+      <c r="P5" s="143"/>
+      <c r="Q5" s="144"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="148"/>
-      <c r="C6" s="149"/>
-      <c r="D6" s="149"/>
-      <c r="E6" s="149"/>
-      <c r="F6" s="149"/>
-      <c r="G6" s="149"/>
-      <c r="H6" s="149"/>
-      <c r="I6" s="149"/>
-      <c r="J6" s="149"/>
-      <c r="K6" s="149"/>
-      <c r="L6" s="149"/>
-      <c r="M6" s="149"/>
-      <c r="N6" s="149"/>
-      <c r="O6" s="149"/>
-      <c r="P6" s="149"/>
-      <c r="Q6" s="150"/>
+      <c r="B6" s="145"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="146"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="146"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="146"/>
+      <c r="L6" s="146"/>
+      <c r="M6" s="146"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="146"/>
+      <c r="P6" s="146"/>
+      <c r="Q6" s="147"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -3613,13 +3734,13 @@
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="151" t="s">
+      <c r="B36" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="151"/>
-      <c r="D36" s="151"/>
-      <c r="E36" s="151"/>
-      <c r="F36" s="151"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
       <c r="H36" s="18" t="s">
         <v>12</v>
       </c>
@@ -3782,13 +3903,13 @@
       <c r="L44" s="123"/>
     </row>
     <row r="45" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="152" t="s">
+      <c r="B45" s="149" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="152"/>
-      <c r="D45" s="152"/>
-      <c r="E45" s="152"/>
-      <c r="F45" s="153">
+      <c r="C45" s="149"/>
+      <c r="D45" s="149"/>
+      <c r="E45" s="149"/>
+      <c r="F45" s="150">
         <f>INDEX(C39:F42,4,3)</f>
         <v>5.8</v>
       </c>
@@ -3803,11 +3924,11 @@
       <c r="L45" s="123"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="152"/>
-      <c r="C46" s="152"/>
-      <c r="D46" s="152"/>
-      <c r="E46" s="152"/>
-      <c r="F46" s="153"/>
+      <c r="B46" s="149"/>
+      <c r="C46" s="149"/>
+      <c r="D46" s="149"/>
+      <c r="E46" s="149"/>
+      <c r="F46" s="150"/>
       <c r="H46" s="117"/>
       <c r="I46" s="22">
         <v>3</v>
@@ -3819,11 +3940,11 @@
       <c r="L46" s="123"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="152"/>
-      <c r="C47" s="152"/>
-      <c r="D47" s="152"/>
-      <c r="E47" s="152"/>
-      <c r="F47" s="153"/>
+      <c r="B47" s="149"/>
+      <c r="C47" s="149"/>
+      <c r="D47" s="149"/>
+      <c r="E47" s="149"/>
+      <c r="F47" s="150"/>
       <c r="H47" s="118"/>
       <c r="I47" s="22">
         <v>4</v>
@@ -3840,21 +3961,21 @@
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="154" t="s">
+      <c r="B52" s="151" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="154"/>
-      <c r="D52" s="154"/>
-      <c r="E52" s="154"/>
-      <c r="F52" s="154"/>
+      <c r="C52" s="151"/>
+      <c r="D52" s="151"/>
+      <c r="E52" s="151"/>
+      <c r="F52" s="151"/>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J53" s="155" t="s">
+      <c r="J53" s="152" t="s">
         <v>33</v>
       </c>
-      <c r="K53" s="155"/>
-      <c r="L53" s="155"/>
-      <c r="M53" s="155"/>
+      <c r="K53" s="152"/>
+      <c r="L53" s="152"/>
+      <c r="M53" s="152"/>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54" s="123"/>
@@ -3872,20 +3993,20 @@
       <c r="H54" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J54" s="156">
+      <c r="J54" s="153">
         <f>INDEX(E55:H58,MATCH(D61,B55:B58,0),MATCH(D62,E54:H54,0))</f>
         <v>2.5</v>
       </c>
-      <c r="K54" s="157"/>
-      <c r="L54" s="157"/>
-      <c r="M54" s="157"/>
+      <c r="K54" s="154"/>
+      <c r="L54" s="154"/>
+      <c r="M54" s="154"/>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B55" s="158" t="s">
+      <c r="B55" s="155" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="158"/>
-      <c r="D55" s="158"/>
+      <c r="C55" s="155"/>
+      <c r="D55" s="155"/>
       <c r="E55" s="21">
         <v>1.5</v>
       </c>
@@ -3901,17 +4022,17 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J55" s="157"/>
-      <c r="K55" s="157"/>
-      <c r="L55" s="157"/>
-      <c r="M55" s="157"/>
+      <c r="J55" s="154"/>
+      <c r="K55" s="154"/>
+      <c r="L55" s="154"/>
+      <c r="M55" s="154"/>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B56" s="158" t="s">
+      <c r="B56" s="155" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="158"/>
-      <c r="D56" s="158"/>
+      <c r="C56" s="155"/>
+      <c r="D56" s="155"/>
       <c r="E56" s="21">
         <v>2</v>
       </c>
@@ -3927,17 +4048,17 @@
         <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
-      <c r="J56" s="157"/>
-      <c r="K56" s="157"/>
-      <c r="L56" s="157"/>
-      <c r="M56" s="157"/>
+      <c r="J56" s="154"/>
+      <c r="K56" s="154"/>
+      <c r="L56" s="154"/>
+      <c r="M56" s="154"/>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B57" s="158" t="s">
+      <c r="B57" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="C57" s="158"/>
-      <c r="D57" s="158"/>
+      <c r="C57" s="155"/>
+      <c r="D57" s="155"/>
       <c r="E57" s="21">
         <v>3.2</v>
       </c>
@@ -3953,17 +4074,17 @@
         <f t="shared" si="3"/>
         <v>4.7</v>
       </c>
-      <c r="J57" s="157"/>
-      <c r="K57" s="157"/>
-      <c r="L57" s="157"/>
-      <c r="M57" s="157"/>
+      <c r="J57" s="154"/>
+      <c r="K57" s="154"/>
+      <c r="L57" s="154"/>
+      <c r="M57" s="154"/>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B58" s="158" t="s">
+      <c r="B58" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="158"/>
-      <c r="D58" s="158"/>
+      <c r="C58" s="155"/>
+      <c r="D58" s="155"/>
       <c r="E58" s="21">
         <v>4.8</v>
       </c>
@@ -3979,10 +4100,10 @@
         <f t="shared" si="3"/>
         <v>6.3</v>
       </c>
-      <c r="J58" s="157"/>
-      <c r="K58" s="157"/>
-      <c r="L58" s="157"/>
-      <c r="M58" s="157"/>
+      <c r="J58" s="154"/>
+      <c r="K58" s="154"/>
+      <c r="L58" s="154"/>
+      <c r="M58" s="154"/>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C60" s="1" t="s">

</xml_diff>